<commit_message>
Revert "Revert "Revert "24-04-2017"""
This reverts commit 3ada2c3c3c979b44212c553e8b161644fb9ce975.
</commit_message>
<xml_diff>
--- a/Mødeprotokol.xlsx
+++ b/Mødeprotokol.xlsx
@@ -114,6 +114,9 @@
     <t>Kom ikke / Syg</t>
   </si>
   <si>
+    <t>Mødt / Smuttet 13:05</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kom ikke / indbrud </t>
   </si>
   <si>
@@ -130,9 +133,6 @@
   </si>
   <si>
     <t>Forsinket / 10:21</t>
-  </si>
-  <si>
-    <t>Forsinket / 11:40</t>
   </si>
 </sst>
 </file>
@@ -332,671 +332,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="77">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666666"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF666666"/>
-          <bgColor rgb="FF666666"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666666"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF666666"/>
-          <bgColor rgb="FF666666"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666666"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF666666"/>
-          <bgColor rgb="FF666666"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666666"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF666666"/>
-          <bgColor rgb="FF666666"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666666"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF666666"/>
-          <bgColor rgb="FF666666"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666666"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF666666"/>
-          <bgColor rgb="FF666666"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666666"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF666666"/>
-          <bgColor rgb="FF666666"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666666"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF666666"/>
-          <bgColor rgb="FF666666"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <font>
         <b val="0"/>
@@ -1465,20 +801,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I112" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I112" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I112"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Uge.Nr" dataDxfId="56">
+    <tableColumn id="1" name="Uge.Nr" dataDxfId="8">
       <calculatedColumnFormula>WEEKNUM(Table1[[#This Row],[Dato]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Dato" dataDxfId="55"/>
-    <tableColumn id="3" name="Casper L" dataDxfId="54"/>
-    <tableColumn id="4" name="Casper S" dataDxfId="53"/>
-    <tableColumn id="5" name="Kasper" dataDxfId="52"/>
-    <tableColumn id="6" name="Lasse" dataDxfId="51"/>
-    <tableColumn id="7" name="Mark" dataDxfId="50"/>
-    <tableColumn id="8" name="Rasmus" dataDxfId="49"/>
-    <tableColumn id="9" name="Mustafa" dataDxfId="48"/>
+    <tableColumn id="2" name="Dato" dataDxfId="7"/>
+    <tableColumn id="3" name="Casper L" dataDxfId="6"/>
+    <tableColumn id="4" name="Casper S" dataDxfId="5"/>
+    <tableColumn id="5" name="Kasper" dataDxfId="4"/>
+    <tableColumn id="6" name="Lasse" dataDxfId="3"/>
+    <tableColumn id="7" name="Mark" dataDxfId="2"/>
+    <tableColumn id="8" name="Rasmus" dataDxfId="1"/>
+    <tableColumn id="9" name="Mustafa" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1784,10 +1120,10 @@
   <dimension ref="A1:J112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I84" sqref="I84"/>
+      <selection pane="bottomRight" activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2635,7 +1971,7 @@
         <v>2</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -2869,7 +2205,7 @@
         <v>2</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>2</v>
@@ -3052,7 +2388,7 @@
         <v>2</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>2</v>
@@ -3073,7 +2409,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>2</v>
@@ -3133,7 +2469,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>2</v>
@@ -3352,7 +2688,7 @@
         <v>2</v>
       </c>
       <c r="H52" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I52" s="3" t="s">
         <v>2</v>
@@ -3382,7 +2718,7 @@
         <v>2</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>2</v>
@@ -4147,25 +3483,25 @@
         <v>42844</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -4177,25 +3513,25 @@
         <v>42845</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -4207,25 +3543,25 @@
         <v>42846</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4297,25 +3633,25 @@
         <v>42849</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5160,62 +4496,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:I22 C23 F23 C24:I51 C52:G52 I52 C53:I63 C64:F64 H64:I64 C65:I112">
-    <cfRule type="containsText" dxfId="76" priority="19" operator="containsText" text="Aftalt">
+    <cfRule type="containsText" dxfId="28" priority="19" operator="containsText" text="Aftalt">
       <formula>NOT(ISERROR(SEARCH("Aftalt",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="20" operator="containsText" text="Mødt">
+    <cfRule type="containsText" dxfId="27" priority="20" operator="containsText" text="Mødt">
       <formula>NOT(ISERROR(SEARCH(("Mødt"),(C1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="21" operator="containsText" text="Kom ikke">
+    <cfRule type="containsText" dxfId="26" priority="21" operator="containsText" text="Kom ikke">
       <formula>NOT(ISERROR(SEARCH(("Kom ikke"),(C1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="22" operator="containsText" text="forsinket">
+    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="forsinket">
       <formula>NOT(ISERROR(SEARCH(("forsinket"),(C1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="23" operator="containsText" text="Weekend">
+    <cfRule type="containsText" dxfId="24" priority="23" operator="containsText" text="Weekend">
       <formula>NOT(ISERROR(SEARCH(("Weekend"),(C1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="24" operator="containsText" text="Ikke registreret">
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="Ikke registreret">
       <formula>NOT(ISERROR(SEARCH(("Ikke registreret"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="containsText" dxfId="70" priority="13" operator="containsText" text="Aftalt">
+    <cfRule type="containsText" dxfId="22" priority="13" operator="containsText" text="Aftalt">
       <formula>NOT(ISERROR(SEARCH("Aftalt",I23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="14" operator="containsText" text="Mødt">
+    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="Mødt">
       <formula>NOT(ISERROR(SEARCH(("Mødt"),(I23))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="15" operator="containsText" text="Kom ikke">
+    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="Kom ikke">
       <formula>NOT(ISERROR(SEARCH(("Kom ikke"),(I23))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="16" operator="containsText" text="forsinket">
+    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="forsinket">
       <formula>NOT(ISERROR(SEARCH(("forsinket"),(I23))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="17" operator="containsText" text="Weekend">
+    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="Weekend">
       <formula>NOT(ISERROR(SEARCH(("Weekend"),(I23))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="18" operator="containsText" text="Ikke registreret">
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="Ikke registreret">
       <formula>NOT(ISERROR(SEARCH(("Ikke registreret"),(I23))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G64">
-    <cfRule type="containsText" dxfId="64" priority="1" operator="containsText" text="Aftalt">
+    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="Aftalt">
       <formula>NOT(ISERROR(SEARCH("Aftalt",G64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="2" operator="containsText" text="Mødt">
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="Mødt">
       <formula>NOT(ISERROR(SEARCH(("Mødt"),(G64))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="3" operator="containsText" text="Kom ikke">
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Kom ikke">
       <formula>NOT(ISERROR(SEARCH(("Kom ikke"),(G64))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="4" operator="containsText" text="forsinket">
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="forsinket">
       <formula>NOT(ISERROR(SEARCH(("forsinket"),(G64))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="5" operator="containsText" text="Weekend">
+    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Weekend">
       <formula>NOT(ISERROR(SEARCH(("Weekend"),(G64))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="6" operator="containsText" text="Ikke registreret">
+    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Ikke registreret">
       <formula>NOT(ISERROR(SEARCH(("Ikke registreret"),(G64))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5276,27 +4612,27 @@
       </c>
       <c r="B2" s="7">
         <f>COUNTIF('Fremmøde Stats'!C2:C112, J2)</f>
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" s="7">
         <f>COUNTIF('Fremmøde Stats'!D2:D112, J2)</f>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" s="7">
         <f>COUNTIF('Fremmøde Stats'!E2:E112, J2)</f>
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E2" s="7">
         <f>COUNTIF('Fremmøde Stats'!F2:F112, J2)</f>
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F2" s="7">
         <f>COUNTIF('Fremmøde Stats'!G2:G112, J2)</f>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G2" s="7">
         <f>COUNTIF('Fremmøde Stats'!H2:H112, J2)</f>
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H2" s="7">
         <f>COUNTIF('Fremmøde Stats'!I2:I112, J2)</f>
@@ -5304,7 +4640,7 @@
       </c>
       <c r="I2" s="7">
         <f t="shared" ref="I2:I4" si="0">SUM(B2:H2)</f>
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "24-04-2017""""
This reverts commit f493cf086a30311cb7b1cb7ea994cec6ba9c1b1e.
</commit_message>
<xml_diff>
--- a/Mødeprotokol.xlsx
+++ b/Mødeprotokol.xlsx
@@ -114,9 +114,6 @@
     <t>Kom ikke / Syg</t>
   </si>
   <si>
-    <t>Mødt / Smuttet 13:05</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kom ikke / indbrud </t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Forsinket / 10:21</t>
+  </si>
+  <si>
+    <t>Forsinket / 11:40</t>
   </si>
 </sst>
 </file>
@@ -332,7 +332,671 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="77">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF666666"/>
+          <bgColor rgb="FF666666"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF666666"/>
+          <bgColor rgb="FF666666"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF666666"/>
+          <bgColor rgb="FF666666"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF666666"/>
+          <bgColor rgb="FF666666"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF666666"/>
+          <bgColor rgb="FF666666"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF666666"/>
+          <bgColor rgb="FF666666"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF666666"/>
+          <bgColor rgb="FF666666"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF666666"/>
+          <bgColor rgb="FF666666"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -801,20 +1465,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I112" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I112" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A1:I112"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Uge.Nr" dataDxfId="8">
+    <tableColumn id="1" name="Uge.Nr" dataDxfId="56">
       <calculatedColumnFormula>WEEKNUM(Table1[[#This Row],[Dato]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Dato" dataDxfId="7"/>
-    <tableColumn id="3" name="Casper L" dataDxfId="6"/>
-    <tableColumn id="4" name="Casper S" dataDxfId="5"/>
-    <tableColumn id="5" name="Kasper" dataDxfId="4"/>
-    <tableColumn id="6" name="Lasse" dataDxfId="3"/>
-    <tableColumn id="7" name="Mark" dataDxfId="2"/>
-    <tableColumn id="8" name="Rasmus" dataDxfId="1"/>
-    <tableColumn id="9" name="Mustafa" dataDxfId="0"/>
+    <tableColumn id="2" name="Dato" dataDxfId="55"/>
+    <tableColumn id="3" name="Casper L" dataDxfId="54"/>
+    <tableColumn id="4" name="Casper S" dataDxfId="53"/>
+    <tableColumn id="5" name="Kasper" dataDxfId="52"/>
+    <tableColumn id="6" name="Lasse" dataDxfId="51"/>
+    <tableColumn id="7" name="Mark" dataDxfId="50"/>
+    <tableColumn id="8" name="Rasmus" dataDxfId="49"/>
+    <tableColumn id="9" name="Mustafa" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1120,10 +1784,10 @@
   <dimension ref="A1:J112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I79" sqref="I79"/>
+      <selection pane="bottomRight" activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1971,7 +2635,7 @@
         <v>2</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -2205,7 +2869,7 @@
         <v>2</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>2</v>
@@ -2388,7 +3052,7 @@
         <v>2</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>2</v>
@@ -2409,7 +3073,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>2</v>
@@ -2469,7 +3133,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>2</v>
@@ -2688,7 +3352,7 @@
         <v>2</v>
       </c>
       <c r="H52" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I52" s="3" t="s">
         <v>2</v>
@@ -2718,7 +3382,7 @@
         <v>2</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>2</v>
@@ -3483,25 +4147,25 @@
         <v>42844</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -3513,25 +4177,25 @@
         <v>42845</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -3543,25 +4207,25 @@
         <v>42846</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3633,25 +4297,25 @@
         <v>42849</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4496,62 +5160,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:I22 C23 F23 C24:I51 C52:G52 I52 C53:I63 C64:F64 H64:I64 C65:I112">
-    <cfRule type="containsText" dxfId="28" priority="19" operator="containsText" text="Aftalt">
+    <cfRule type="containsText" dxfId="76" priority="19" operator="containsText" text="Aftalt">
       <formula>NOT(ISERROR(SEARCH("Aftalt",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="20" operator="containsText" text="Mødt">
+    <cfRule type="containsText" dxfId="75" priority="20" operator="containsText" text="Mødt">
       <formula>NOT(ISERROR(SEARCH(("Mødt"),(C1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="21" operator="containsText" text="Kom ikke">
+    <cfRule type="containsText" dxfId="74" priority="21" operator="containsText" text="Kom ikke">
       <formula>NOT(ISERROR(SEARCH(("Kom ikke"),(C1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="forsinket">
+    <cfRule type="containsText" dxfId="73" priority="22" operator="containsText" text="forsinket">
       <formula>NOT(ISERROR(SEARCH(("forsinket"),(C1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="23" operator="containsText" text="Weekend">
+    <cfRule type="containsText" dxfId="72" priority="23" operator="containsText" text="Weekend">
       <formula>NOT(ISERROR(SEARCH(("Weekend"),(C1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="Ikke registreret">
+    <cfRule type="containsText" dxfId="71" priority="24" operator="containsText" text="Ikke registreret">
       <formula>NOT(ISERROR(SEARCH(("Ikke registreret"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="containsText" dxfId="22" priority="13" operator="containsText" text="Aftalt">
+    <cfRule type="containsText" dxfId="70" priority="13" operator="containsText" text="Aftalt">
       <formula>NOT(ISERROR(SEARCH("Aftalt",I23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="Mødt">
+    <cfRule type="containsText" dxfId="69" priority="14" operator="containsText" text="Mødt">
       <formula>NOT(ISERROR(SEARCH(("Mødt"),(I23))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="Kom ikke">
+    <cfRule type="containsText" dxfId="68" priority="15" operator="containsText" text="Kom ikke">
       <formula>NOT(ISERROR(SEARCH(("Kom ikke"),(I23))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="forsinket">
+    <cfRule type="containsText" dxfId="67" priority="16" operator="containsText" text="forsinket">
       <formula>NOT(ISERROR(SEARCH(("forsinket"),(I23))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="Weekend">
+    <cfRule type="containsText" dxfId="66" priority="17" operator="containsText" text="Weekend">
       <formula>NOT(ISERROR(SEARCH(("Weekend"),(I23))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="Ikke registreret">
+    <cfRule type="containsText" dxfId="65" priority="18" operator="containsText" text="Ikke registreret">
       <formula>NOT(ISERROR(SEARCH(("Ikke registreret"),(I23))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G64">
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="Aftalt">
+    <cfRule type="containsText" dxfId="64" priority="1" operator="containsText" text="Aftalt">
       <formula>NOT(ISERROR(SEARCH("Aftalt",G64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="Mødt">
+    <cfRule type="containsText" dxfId="63" priority="2" operator="containsText" text="Mødt">
       <formula>NOT(ISERROR(SEARCH(("Mødt"),(G64))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Kom ikke">
+    <cfRule type="containsText" dxfId="62" priority="3" operator="containsText" text="Kom ikke">
       <formula>NOT(ISERROR(SEARCH(("Kom ikke"),(G64))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="forsinket">
+    <cfRule type="containsText" dxfId="61" priority="4" operator="containsText" text="forsinket">
       <formula>NOT(ISERROR(SEARCH(("forsinket"),(G64))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Weekend">
+    <cfRule type="containsText" dxfId="60" priority="5" operator="containsText" text="Weekend">
       <formula>NOT(ISERROR(SEARCH(("Weekend"),(G64))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Ikke registreret">
+    <cfRule type="containsText" dxfId="59" priority="6" operator="containsText" text="Ikke registreret">
       <formula>NOT(ISERROR(SEARCH(("Ikke registreret"),(G64))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4612,27 +5276,27 @@
       </c>
       <c r="B2" s="7">
         <f>COUNTIF('Fremmøde Stats'!C2:C112, J2)</f>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C2" s="7">
         <f>COUNTIF('Fremmøde Stats'!D2:D112, J2)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" s="7">
         <f>COUNTIF('Fremmøde Stats'!E2:E112, J2)</f>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E2" s="7">
         <f>COUNTIF('Fremmøde Stats'!F2:F112, J2)</f>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F2" s="7">
         <f>COUNTIF('Fremmøde Stats'!G2:G112, J2)</f>
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G2" s="7">
         <f>COUNTIF('Fremmøde Stats'!H2:H112, J2)</f>
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H2" s="7">
         <f>COUNTIF('Fremmøde Stats'!I2:I112, J2)</f>
@@ -4640,7 +5304,7 @@
       </c>
       <c r="I2" s="7">
         <f t="shared" ref="I2:I4" si="0">SUM(B2:H2)</f>
-        <v>276</v>
+        <v>293</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>9</v>

</xml_diff>